<commit_message>
add filter and redo undo test case
</commit_message>
<xml_diff>
--- a/src/main/resources/data/loadData.xlsx
+++ b/src/main/resources/data/loadData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
   <si>
     <t>title</t>
   </si>
@@ -71,6 +71,30 @@
   </si>
   <si>
     <t>{}</t>
+  </si>
+  <si>
+    <t>图分析视图-loadData-跨账号不载入数据</t>
+  </si>
+  <si>
+    <t>{"projectId":1334,"graphId":2497,"fileName":"graphTestData.json"}</t>
+  </si>
+  <si>
+    <t>无权访问</t>
+  </si>
+  <si>
+    <t>图分析视图-loadData-同账号非当前项目标签不能载入数据</t>
+  </si>
+  <si>
+    <t>{"projectId":1426,"graphId":2827,"fileName":"graphTestData.json"}</t>
+  </si>
+  <si>
+    <t>无权操作</t>
+  </si>
+  <si>
+    <t>图分析视图-loadData-项目下不存在的标签不能载入数据</t>
+  </si>
+  <si>
+    <t>{"projectId":1426,"graphId":2772,"fileName":"graphTestData.json"}</t>
   </si>
 </sst>
 </file>
@@ -78,10 +102,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -118,9 +142,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -132,6 +163,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,48 +226,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,19 +250,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -216,57 +278,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -289,13 +313,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,13 +415,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,151 +487,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,11 +582,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,6 +602,45 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,56 +671,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,148 +684,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2020,7 +2044,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="5"/>
@@ -2101,7 +2125,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="9"/>
     </row>
@@ -2119,7 +2143,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="9"/>
     </row>
@@ -2137,32 +2161,62 @@
         <v>14</v>
       </c>
       <c r="E6" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" ht="20.05" customHeight="1" spans="1:6">
-      <c r="A7" s="12"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+    <row r="7" s="1" customFormat="1" ht="20.05" customHeight="1" spans="1:6">
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="9">
+        <v>401</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" ht="20.05" customHeight="1" spans="1:6">
-      <c r="A8" s="12"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+    <row r="8" s="1" customFormat="1" ht="20.05" customHeight="1" spans="1:6">
+      <c r="A8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9">
+        <v>90009</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" ht="20.05" customHeight="1" spans="1:6">
-      <c r="A9" s="12"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+    <row r="9" s="1" customFormat="1" ht="20.05" customHeight="1" spans="1:6">
+      <c r="A9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="9">
+        <v>90009</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
       <c r="F9" s="9"/>
     </row>
     <row r="10" ht="20.05" customHeight="1" spans="1:6">

</xml_diff>